<commit_message>
Added Git slides, made formatting consistent, Updated lesson 4 with PR information
</commit_message>
<xml_diff>
--- a/Lesson Info.xlsx
+++ b/Lesson Info.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2501f1c4df9ee7ad/Documents/Code The Dream/intro-to-programming-2026/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_F25DC773A252ABDACC1048C9E19D41B45ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{678EE18F-E795-48D4-A22B-AEC58EB95F76}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="11_F25DC773A252ABDACC1048C9E19D41B45ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EAC1F885-A19F-413D-A436-BB640235858E}"/>
   <bookViews>
-    <workbookView xWindow="5004" yWindow="600" windowWidth="21180" windowHeight="14292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2520" yWindow="1980" windowWidth="23160" windowHeight="14292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -48,26 +57,6 @@
     <t>Lesson 2</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Gain an understanding of what JavaScript is and where it is used.
- - Learn the basic syntax rules of JavaScript
- - Understand what variables, data types, conditional statements, and functions are and how they are used
- - Begin to learn and work with ways of troubleshooting problems
- - Learn what functions are, how they are written, and the benefits of their use
- - Understand how data can be passed to a function to use inside the function
- - Learn what arrow functions are and when and why they are used</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Learn the syntax and value of using loops for repetitive tasks
- - Practice writing and working with 'for' loops to avoid infinite loops
- - Learn about the structure and purpose of arrays</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Learn what an object is and how it is written
- - Understand the difference between primitive and object data types
- - Practice destructuring objects so you can work with individual values within an object
- - Manipulate objects to see how they can be changed or amended</t>
-  </si>
-  <si>
     <t>Lesson 3</t>
   </si>
   <si>
@@ -75,13 +64,6 @@
   </si>
   <si>
     <t>Lesson 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - Use methods on arrays to understand how arrays and/or parts of their can be manipulated or worked with
- - Begin learning about iterative methods that can work with each item within an array
- - Learn the structuring of callback functions and the logic of running one function after another so as to work with results of the first
- - Start creating higher order functions that accept functions as parameters or return functions
- - Use existing higher order array functions to iterate through arrays (examples include forEach, map, and filter to name a few)</t>
   </si>
   <si>
     <t xml:space="preserve"> - Learn a brief history of the internet and the web and how the web works
@@ -112,6 +94,29 @@
   </si>
   <si>
     <t>https://raw.githubusercontent.com/Code-the-Dream-School/intro-to-programming-2026/refs/heads/main/assignments/Assignment%2004%20-%20JavaScript%20Algorithms.md</t>
+  </si>
+  <si>
+    <t>- Problem Solving
+- Javascript Basics: Variables, Strings, Types, Conditions and Function
+- Debugging Basics
+- Console / Terminals
+- Software Repositories / Github</t>
+  </si>
+  <si>
+    <t>- Javascript Loops 
+- Javascript Arrays 
+- Scope
+- Version Control Systems / Git</t>
+  </si>
+  <si>
+    <t>- Javascript Objects
+- Continuing with Git - Commit and Push Objects</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Algorithms
+ - Pseudocode
+ - Learn the structuring of callback functions and the logic of running one function after another so as to work with results of the first
+ - Continuing with Git  - What is a Pull Request</t>
   </si>
 </sst>
 </file>
@@ -193,6 +198,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -460,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,12 +484,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -496,7 +505,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -504,12 +513,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -525,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -533,15 +542,15 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>9</v>
+      <c r="B13" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -549,7 +558,7 @@
         <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -557,20 +566,20 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -578,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -586,12 +595,12 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="144" x14ac:dyDescent="0.3">
@@ -599,7 +608,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -614,8 +623,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{279ACCA6-943A-4609-B4A9-277301C6BCEE}"/>
-    <hyperlink ref="B9" r:id="rId2" xr:uid="{A0EB65CC-0AE5-48B2-8D24-B971DF8A3129}"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{A0EB65CC-0AE5-48B2-8D24-B971DF8A3129}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{279ACCA6-943A-4609-B4A9-277301C6BCEE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>

</xml_diff>

<commit_message>
Updated lessons  and assignment links
</commit_message>
<xml_diff>
--- a/Lesson Info.xlsx
+++ b/Lesson Info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2501f1c4df9ee7ad/Documents/Code The Dream/intro-to-programming-2026/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="11_F25DC773A252ABDACC1048C9E19D41B45ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D31EF60-3172-40F2-B364-B3816F31965F}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="11_F25DC773A252ABDACC1048C9E19D41B45ADE58F3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E734613E-35B9-483D-A448-08F9CBF448FF}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="480" windowWidth="23160" windowHeight="14292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4380" yWindow="804" windowWidth="21432" windowHeight="14136" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="47">
   <si>
     <t>Learning Objectives</t>
   </si>
@@ -66,18 +66,6 @@
     <t>Lesson 5</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Learn a brief history of the internet and the web and how the web works
- - Learn the structure and format of URLs
- - Understand what domain names, IP addresses, and the Domain Name System are and begin to see how IP addresses are used with domain names
- - Find out what HTTP and HTTPS mean, the differences between them, and how they are used
- - Begin learning about and practice writing HTML (Hypertext Markup Language)
- - Practice formatting page content using HTML and learn about inline versus block level elements
- - Understand and work with file paths to see how files in different locations can be referenced or used within another file
- - Learn how to display visual content like images in an HTML file
- - Find out what HTML elements can help create and work with forms to allow a user to provide data using input elements
- - Get an introduction to Web Accessibility basics which allow a web page to reach more people</t>
-  </si>
-  <si>
     <t>https://raw.githubusercontent.com/Code-the-Dream-School/intro-to-programming-2026/refs/heads/main/lessons/Lesson%2003%20-%20Javascript%20Objects.md</t>
   </si>
   <si>
@@ -96,34 +84,116 @@
     <t>https://raw.githubusercontent.com/Code-the-Dream-School/intro-to-programming-2026/refs/heads/main/assignments/Assignment%2004%20-%20JavaScript%20Algorithms.md</t>
   </si>
   <si>
-    <t>- Problem Solving
-- Javascript Basics: Variables, Strings, Types, Conditions and Function
-- Debugging Basics
-- Console / Terminals
-- Software Repositories / Github</t>
-  </si>
-  <si>
-    <t>- Javascript Loops 
-- Javascript Arrays 
-- Scope
-- Version Control Systems / Git</t>
-  </si>
-  <si>
-    <t>- Javascript Objects
-- Continuing with Git - Commit and Push Objects</t>
+    <t>Lesson 6</t>
+  </si>
+  <si>
+    <t>Lesson 7</t>
+  </si>
+  <si>
+    <t>Lesson 8</t>
+  </si>
+  <si>
+    <t>Lesson 9</t>
+  </si>
+  <si>
+    <t>Lesson 10</t>
+  </si>
+  <si>
+    <t>Lesson 11</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/assignments/Assignment%2006%20-%20CSS%20Basics.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/assignments/Assignment%2007%20-%20The%20DOM%20API.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/assignments/Assignment%2008%20-%20Async%20Programming%20and%20Promises.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/assignments/Assignment%2009%20-%20Fetch%20API.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/assignments/Assignment%2010%20-%20Open%20API.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/assignments/Assignment%2011%20-%20Final%20Project.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/assignments/Assignment%2005%20-%20HTML%20Basics.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/lessons/Lesson%2005%20-%20HTML%20Basics.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/lessons/Lesson%2006%20-%20CSS%20Basics.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/lessons/Lesson%2007%20-%20The%20DOM%20API.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/lessons/Lesson%2008%20-%20Async%20Programming%20and%20Promises.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/lessons/Lesson%2009%20-%20Fetch%20API.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/TeresaSwarthout/intro-to-programming-2026/refs/heads/main/lessons/Lesson%2010%20-%20Open%20API.md</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Code-the-Dream-School/intro-to-programming-2026/refs/heads/main/assignments/Assignment%2011%20-%20Final%20Project.md</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Javascript Basics
+ - Javascript Variables, Data Types, Conditional Statements and Functions
+ - Basic Debugging and Problem Solving
+ - Software Repositories</t>
+  </si>
+  <si>
+    <t>- Javascript Objecs
+- Continuing with Git Usage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Javascript Loops and Arrays
+ - Scope
+ - Version Control Systems</t>
   </si>
   <si>
     <t xml:space="preserve"> - Algorithms
  - Pseudocode
- - Learn the structuring of callback functions and the logic of running one function after another so as to work with results of the first
- - Continuing with Git  - What is a Pull Request</t>
+ - Continuing with Git  - Pull Request?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - How Does the Web Work?
+ - Introduction to HTML and CSS
+ - HTML Basics
+ - Integrated Development Environments / Visual Studio Code</t>
+  </si>
+  <si>
+    <t>- CSS Basics</t>
+  </si>
+  <si>
+    <t>- The DOM (Document Object Model)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - The Fetch API</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Async Programming and Promises
+ - Synchronous vs Asynchronous Code</t>
+  </si>
+  <si>
+    <t>- Open APIs</t>
+  </si>
+  <si>
+    <t>- Final Project</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,14 +205,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -165,13 +227,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
@@ -182,9 +242,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B25"/>
+  <dimension ref="A2:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,145 +540,326 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="5" t="s">
+    <row r="38" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" s="4" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="144" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>1</v>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>